<commit_message>
Add toolchain 4.0.4 extension list and mcpu list
</commit_message>
<xml_diff>
--- a/mcpu_lists/compiler-mcpu.xlsx
+++ b/mcpu_lists/compiler-mcpu.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O87"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
@@ -461,6 +461,8 @@
     <col customWidth="1" max="13" min="13" width="15.6"/>
     <col customWidth="1" max="14" min="14" width="13.2"/>
     <col customWidth="1" max="15" min="15" width="15.6"/>
+    <col customWidth="1" max="16" min="16" width="13.2"/>
+    <col customWidth="1" max="17" min="17" width="15.6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -539,6 +541,16 @@
           <t>4.0.3-Clang</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>4.0.4-GCC</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>4.0.4-Clang</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -588,6 +600,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -637,6 +655,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -682,6 +706,12 @@
       </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -723,6 +753,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -772,6 +808,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -821,6 +863,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -866,6 +914,12 @@
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -907,6 +961,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -956,6 +1016,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1005,6 +1071,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1054,6 +1126,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1103,6 +1181,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1148,6 +1232,12 @@
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -1185,6 +1275,8 @@
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1246,6 +1338,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1323,6 +1425,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1400,6 +1512,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1477,6 +1599,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1554,6 +1686,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1631,6 +1773,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1708,6 +1860,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1785,6 +1947,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1862,6 +2034,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1939,6 +2121,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2016,6 +2208,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2093,6 +2295,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2170,6 +2382,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2247,6 +2469,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2320,6 +2552,16 @@
         </is>
       </c>
       <c r="O30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2385,6 +2627,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2442,6 +2694,16 @@
         </is>
       </c>
       <c r="O32" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2483,6 +2745,8 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2560,6 +2824,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2637,6 +2911,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2686,6 +2970,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2763,6 +3053,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2836,6 +3136,16 @@
         </is>
       </c>
       <c r="O38" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -2865,6 +3175,8 @@
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2914,6 +3226,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2991,6 +3309,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3040,6 +3368,12 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3117,6 +3451,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3190,6 +3534,16 @@
         </is>
       </c>
       <c r="O44" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -3219,6 +3573,8 @@
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3244,6 +3600,8 @@
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3321,6 +3679,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3398,6 +3766,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3475,6 +3853,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3552,6 +3940,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3629,6 +4027,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3706,6 +4114,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3783,6 +4201,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3860,6 +4288,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3937,6 +4375,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4010,6 +4458,16 @@
         </is>
       </c>
       <c r="O56" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4039,6 +4497,8 @@
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4068,6 +4528,8 @@
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4145,6 +4607,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4222,6 +4694,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4299,6 +4781,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4376,6 +4868,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4453,6 +4955,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4530,6 +5042,16 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4603,6 +5125,16 @@
         </is>
       </c>
       <c r="O65" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4652,79 +5184,43 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>sifive-x280</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr">
+          <t>sifive-x180</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q67" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4733,7 +5229,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>sifive-x280n</t>
+          <t>sifive-x280</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -4802,6 +5298,16 @@
         </is>
       </c>
       <c r="O68" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q68" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4810,7 +5316,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>sifive-x280o</t>
+          <t>sifive-x280n</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -4879,6 +5385,16 @@
         </is>
       </c>
       <c r="O69" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q69" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4887,7 +5403,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>sifive-x390</t>
+          <t>sifive-x280o</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -4895,7 +5411,11 @@
           <t>X</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D70" t="inlineStr">
         <is>
           <t>X</t>
@@ -4952,6 +5472,16 @@
         </is>
       </c>
       <c r="O70" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q70" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -4960,39 +5490,81 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>sifive-x390-fast-fp64</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
+          <t>sifive-x390</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
-      <c r="F71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="G71" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="I71" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="J71" t="inlineStr"/>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="K71" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr"/>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="M71" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="N71" t="inlineStr"/>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="O71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q71" t="inlineStr">
         <is>
           <t>X</t>
         </is>
@@ -5001,36 +5573,54 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>sifive-x392-ea-dualvalu</t>
+          <t>sifive-x390-fast-fp64</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="J72" t="inlineStr"/>
-      <c r="K72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr"/>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>sifive-x392-ea-singlevalu</t>
+          <t>sifive-x392-ea-dualvalu</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -5055,68 +5645,52 @@
       <c r="M73" t="inlineStr"/>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>spacemit-x60</t>
+          <t>sifive-x392-ea-singlevalu</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="K74" t="inlineStr"/>
       <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>syntacore-scr1-base</t>
+          <t>spacemit-x60</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr">
         <is>
@@ -5141,11 +5715,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>syntacore-scr1-max</t>
+          <t>syntacore-scr1-base</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -5190,19 +5770,37 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>syntacore-scr3-rv32</t>
+          <t>syntacore-scr1-max</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr"/>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="F77" t="inlineStr"/>
-      <c r="G77" t="inlineStr"/>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
         <is>
@@ -5227,11 +5825,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>syntacore-scr3-rv64</t>
+          <t>syntacore-scr3-rv32</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -5264,11 +5868,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>syntacore-scr4-rv32</t>
+          <t>syntacore-scr3-rv64</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -5301,11 +5911,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>syntacore-scr4-rv64</t>
+          <t>syntacore-scr4-rv32</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -5338,11 +5954,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>syntacore-scr5-rv32</t>
+          <t>syntacore-scr4-rv64</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -5375,11 +5997,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>syntacore-scr5-rv64</t>
+          <t>syntacore-scr5-rv32</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -5412,11 +6040,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>syntacore-scr7</t>
+          <t>syntacore-scr5-rv64</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -5449,113 +6083,123 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>thead-c906</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+          <t>syntacore-scr7</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr"/>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="O84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>tt-ascalon-d8</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
+          <t>thead-c906</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="E85" t="inlineStr"/>
-      <c r="F85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N85" t="inlineStr"/>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>veyron-v1</t>
+          <t>tt-ascalon-d8</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="inlineStr">
         <is>
@@ -5580,11 +6224,17 @@
           <t>X</t>
         </is>
       </c>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>xiangshan-nanhu</t>
+          <t>veyron-v1</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -5601,116 +6251,187 @@
           <t>X</t>
         </is>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="H87" t="inlineStr"/>
       <c r="I87" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="L87" t="inlineStr"/>
       <c r="M87" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>xiangshan-nanhu</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B87">
+  <conditionalFormatting sqref="B2:B88">
     <cfRule dxfId="0" priority="1" type="expression">
       <formula>$B2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C87">
+  <conditionalFormatting sqref="C2:C88">
     <cfRule dxfId="0" priority="2" type="expression">
       <formula>$C2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D87">
+  <conditionalFormatting sqref="D2:D88">
     <cfRule dxfId="0" priority="3" type="expression">
       <formula>$D2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E87">
+  <conditionalFormatting sqref="E2:E88">
     <cfRule dxfId="0" priority="4" type="expression">
       <formula>$E2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F87">
+  <conditionalFormatting sqref="F2:F88">
     <cfRule dxfId="0" priority="5" type="expression">
       <formula>$F2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G87">
+  <conditionalFormatting sqref="G2:G88">
     <cfRule dxfId="0" priority="6" type="expression">
       <formula>$G2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H87">
+  <conditionalFormatting sqref="H2:H88">
     <cfRule dxfId="0" priority="7" type="expression">
       <formula>$H2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I87">
+  <conditionalFormatting sqref="I2:I88">
     <cfRule dxfId="0" priority="8" type="expression">
       <formula>$I2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J87">
+  <conditionalFormatting sqref="J2:J88">
     <cfRule dxfId="0" priority="9" type="expression">
       <formula>$J2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K87">
+  <conditionalFormatting sqref="K2:K88">
     <cfRule dxfId="0" priority="10" type="expression">
       <formula>$K2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L87">
+  <conditionalFormatting sqref="L2:L88">
     <cfRule dxfId="0" priority="11" type="expression">
       <formula>$L2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M87">
+  <conditionalFormatting sqref="M2:M88">
     <cfRule dxfId="0" priority="12" type="expression">
       <formula>$M2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N87">
+  <conditionalFormatting sqref="N2:N88">
     <cfRule dxfId="0" priority="13" type="expression">
       <formula>$N2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O87">
+  <conditionalFormatting sqref="O2:O88">
     <cfRule dxfId="0" priority="14" type="expression">
       <formula>$O2="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P88">
+    <cfRule dxfId="0" priority="15" type="expression">
+      <formula>$P2="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q88">
+    <cfRule dxfId="0" priority="16" type="expression">
+      <formula>$Q2="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>